<commit_message>
Modified table structure and data
</commit_message>
<xml_diff>
--- a/mcdonoughData.xlsx
+++ b/mcdonoughData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="SIDE" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="340">
   <si>
     <t xml:space="preserve">sideName</t>
   </si>
@@ -106,7 +106,10 @@
     <t xml:space="preserve">zeus x27</t>
   </si>
   <si>
-    <t xml:space="preserve">name</t>
+    <t xml:space="preserve">weaponNum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weaponName</t>
   </si>
   <si>
     <t xml:space="preserve">exclusiveSide</t>
@@ -289,121 +292,25 @@
     <t xml:space="preserve">lose via round expire</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">pistol </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">elimination</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">shotgun </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">elimination</t>
-    </r>
+    <t xml:space="preserve">pistol elimination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shotgun elimination</t>
   </si>
   <si>
     <t xml:space="preserve">light machine gun elimination</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">submachine gun </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">elimination</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">rifle </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">elimination</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">sniper </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">elimination</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">knife </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">elimination</t>
-    </r>
+    <t xml:space="preserve">submachine gun elimination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rifle elimination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sniper elimination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">knife elimination</t>
   </si>
   <si>
     <t xml:space="preserve">bomb plant</t>
@@ -817,7 +724,7 @@
     <t xml:space="preserve">teamNum</t>
   </si>
   <si>
-    <t xml:space="preserve">organization</t>
+    <t xml:space="preserve">teamName</t>
   </si>
   <si>
     <t xml:space="preserve">currentRank</t>
@@ -1154,7 +1061,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1175,11 +1082,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1224,16 +1126,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1257,10 +1155,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.95"/>
   </cols>
@@ -1317,26 +1215,26 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1344,10 +1242,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -1361,10 +1259,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>2</v>
@@ -1378,10 +1276,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>3</v>
@@ -1395,10 +1293,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>4</v>
@@ -1412,10 +1310,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>5</v>
@@ -1429,10 +1327,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>6</v>
@@ -1446,10 +1344,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>7</v>
@@ -1463,10 +1361,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>9</v>
@@ -1480,10 +1378,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>10</v>
@@ -1497,10 +1395,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>11</v>
@@ -1514,13 +1412,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>24</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1528,16 +1429,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>8</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>0</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1545,13 +1446,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>114</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1559,13 +1463,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>33</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1573,10 +1480,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1584,10 +1494,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1595,10 +1508,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1606,13 +1522,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>41</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1620,10 +1539,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1642,13 +1564,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.22"/>
@@ -1656,31 +1578,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1688,13 +1610,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
@@ -1706,10 +1628,10 @@
         <v>250000</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,13 +1639,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>2014</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>2</v>
@@ -1735,10 +1657,10 @@
         <v>250000</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,13 +1668,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2014</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>3</v>
@@ -1764,10 +1686,10 @@
         <v>250000</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1775,13 +1697,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>2014</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1</v>
@@ -1793,10 +1715,10 @@
         <v>250000</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1804,13 +1726,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>2</v>
@@ -1822,10 +1744,10 @@
         <v>250000</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1833,13 +1755,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>3</v>
@@ -1851,10 +1773,10 @@
         <v>250000</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1862,13 +1784,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>4</v>
@@ -1880,10 +1802,10 @@
         <v>1000000</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1891,13 +1813,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>2016</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>5</v>
@@ -1909,10 +1831,10 @@
         <v>1000000</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1920,13 +1842,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>2016</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>3</v>
@@ -1938,10 +1860,10 @@
         <v>1000000</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1949,13 +1871,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>6</v>
@@ -1967,10 +1889,10 @@
         <v>1000000</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1978,13 +1900,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>7</v>
@@ -1996,10 +1918,10 @@
         <v>1000000</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2007,28 +1929,28 @@
         <v>4</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>8</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>1000000</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2036,13 +1958,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>9</v>
@@ -2054,10 +1976,10 @@
         <v>1000000</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2065,13 +1987,13 @@
         <v>2</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>2</v>
@@ -2083,10 +2005,10 @@
         <v>1000000</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2094,13 +2016,13 @@
         <v>7</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>10</v>
@@ -2112,10 +2034,10 @@
         <v>1000000</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2123,28 +2045,28 @@
         <v>2</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>3</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>250000</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2152,13 +2074,13 @@
         <v>2</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>11</v>
@@ -2170,10 +2092,10 @@
         <v>250000</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2181,13 +2103,13 @@
         <v>2</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>2019</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>12</v>
@@ -2199,10 +2121,10 @@
         <v>250000</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2210,13 +2132,13 @@
         <v>8</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>13</v>
@@ -2228,10 +2150,10 @@
         <v>490000</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2239,28 +2161,57 @@
         <v>1</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>14</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>15000</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>250000</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2285,20 +2236,20 @@
       <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2306,13 +2257,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2320,13 +2271,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2334,13 +2285,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2348,13 +2299,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2362,13 +2313,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2376,13 +2327,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2390,13 +2341,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2404,13 +2355,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2418,13 +2369,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2432,13 +2383,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2446,13 +2397,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2460,13 +2411,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2474,13 +2425,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2488,13 +2439,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2519,26 +2470,26 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2546,16 +2497,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1994</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2563,16 +2514,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>2000</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2580,13 +2531,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2002</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2594,16 +2545,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>2016</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2611,16 +2562,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>2002</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2628,13 +2579,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2642,13 +2593,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>2012</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2656,13 +2607,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>2016</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2687,7 +2638,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2797,9 +2748,9 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2864,464 +2815,572 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1050</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1300</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>1100</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1700</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>5200</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>1050</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>1200</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>2350</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>1400</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>1250</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>1800</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>2700</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B27" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>3000</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B28" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>3100</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>3100</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>2050</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>3300</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>1700</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>400</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="D34" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>700</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="D35" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>1050</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>1700</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <v>5200</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>1050</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="0" t="n">
-        <v>1200</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <v>2350</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>1400</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>1250</v>
-      </c>
-      <c r="D23" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>1800</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>2700</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="0" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D27" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="0" t="n">
-        <v>3100</v>
-      </c>
-      <c r="D28" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="0" t="n">
-        <v>3100</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="0" t="n">
-        <v>2050</v>
-      </c>
-      <c r="D30" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="0" t="n">
-        <v>3300</v>
-      </c>
-      <c r="D31" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="0" t="n">
-        <v>4750</v>
-      </c>
-      <c r="D32" s="0" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="0" t="n">
-        <v>1700</v>
-      </c>
-      <c r="D33" s="0" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="0" t="n">
-        <v>5000</v>
-      </c>
-      <c r="D34" s="0" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="0" t="n">
-        <v>5000</v>
-      </c>
-      <c r="D35" s="0" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="0" t="n">
+      <c r="B36" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="E36" s="0" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3347,17 +3406,17 @@
       <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="2" t="s">
         <v>64</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3365,7 +3424,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>11</v>
@@ -3376,7 +3435,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>12</v>
@@ -3387,7 +3446,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>13</v>
@@ -3398,7 +3457,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>14</v>
@@ -3409,7 +3468,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>15</v>
@@ -3420,7 +3479,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>16</v>
@@ -3431,7 +3490,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>17</v>
@@ -3455,11 +3514,11 @@
   </sheetPr>
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.51"/>
@@ -3467,13 +3526,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3481,7 +3540,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1400</v>
@@ -3492,7 +3551,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>1900</v>
@@ -3503,7 +3562,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2400</v>
@@ -3514,7 +3573,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>2900</v>
@@ -3525,7 +3584,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>3400</v>
@@ -3536,7 +3595,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>3250</v>
@@ -3547,7 +3606,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>3500</v>
@@ -3558,7 +3617,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>3600</v>
@@ -3569,7 +3628,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>3250</v>
@@ -3580,7 +3639,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0</v>
@@ -3591,7 +3650,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>300</v>
@@ -3602,7 +3661,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>900</v>
@@ -3613,7 +3672,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>200</v>
@@ -3624,7 +3683,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>600</v>
@@ -3635,7 +3694,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>300</v>
@@ -3646,7 +3705,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>100</v>
@@ -3657,7 +3716,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>1500</v>
@@ -3668,7 +3727,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>800</v>
@@ -3692,39 +3751,39 @@
   </sheetPr>
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3732,22 +3791,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>56</v>
+      <c r="G2" s="0" t="n">
+        <v>30</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>800</v>
@@ -3758,22 +3817,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>104</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>33</v>
+      <c r="G3" s="0" t="n">
+        <v>7</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>720</v>
@@ -3784,22 +3843,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>53</v>
+      <c r="G4" s="0" t="n">
+        <v>27</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>840</v>
@@ -3810,22 +3869,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>111</v>
-      </c>
       <c r="E5" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>56</v>
+      <c r="G5" s="0" t="n">
+        <v>30</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>760</v>
@@ -3836,22 +3895,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>113</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>51</v>
+      <c r="G6" s="0" t="n">
+        <v>25</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>880</v>
@@ -3862,22 +3921,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>113</v>
+        <v>120</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>52</v>
+      <c r="G7" s="0" t="n">
+        <v>26</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>920</v>
@@ -3888,22 +3947,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>30</v>
+      <c r="G8" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>640</v>
@@ -3914,22 +3973,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>124</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>123</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="G9" s="0" t="s">
-        <v>57</v>
+      <c r="G9" s="0" t="n">
+        <v>31</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>880</v>
@@ -3940,22 +3999,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="G10" s="0" t="s">
-        <v>53</v>
+      <c r="G10" s="0" t="n">
+        <v>27</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>680</v>
@@ -3966,22 +4025,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>113</v>
+        <v>133</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="G11" s="0" t="s">
-        <v>56</v>
+      <c r="G11" s="0" t="n">
+        <v>35</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>800</v>
@@ -3992,22 +4051,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E12" s="2" t="s">
         <v>136</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="G12" s="0" t="s">
-        <v>35</v>
+      <c r="G12" s="0" t="n">
+        <v>9</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>560</v>
@@ -4018,22 +4077,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>113</v>
+        <v>140</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="G13" s="0" t="s">
-        <v>52</v>
+      <c r="G13" s="0" t="n">
+        <v>26</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>1240</v>
@@ -4044,22 +4103,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>57</v>
+      <c r="G14" s="1" t="n">
+        <v>31</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>960</v>
@@ -4070,22 +4129,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G15" s="0" t="s">
-        <v>45</v>
+      <c r="G15" s="0" t="n">
+        <v>19</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>960</v>
@@ -4096,22 +4155,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G16" s="0" t="s">
-        <v>51</v>
+      <c r="G16" s="0" t="n">
+        <v>25</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>560</v>
@@ -4122,22 +4181,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="G17" s="0" t="s">
-        <v>33</v>
+      <c r="G17" s="0" t="n">
+        <v>7</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>900</v>
@@ -4148,22 +4207,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>156</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>155</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="G18" s="0" t="s">
-        <v>51</v>
+      <c r="G18" s="0" t="n">
+        <v>25</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>764</v>
@@ -4174,22 +4233,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>57</v>
+      <c r="G19" s="1" t="n">
+        <v>31</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>800</v>
@@ -4200,22 +4259,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="G20" s="0" t="s">
-        <v>32</v>
+      <c r="G20" s="0" t="n">
+        <v>6</v>
       </c>
       <c r="H20" s="0" t="n">
         <v>680</v>
@@ -4226,22 +4285,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="G21" s="0" t="s">
-        <v>58</v>
+      <c r="G21" s="0" t="n">
+        <v>32</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>880</v>
@@ -4252,22 +4311,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="G22" s="0" t="s">
-        <v>51</v>
+      <c r="G22" s="0" t="n">
+        <v>25</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>788</v>
@@ -4278,22 +4337,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>54</v>
+        <v>8</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>28</v>
       </c>
       <c r="H23" s="0" t="n">
         <v>760</v>
@@ -4304,22 +4363,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>55</v>
+        <v>8</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>29</v>
       </c>
       <c r="H24" s="0" t="n">
         <v>320</v>
@@ -4330,22 +4389,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>33</v>
+        <v>8</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>7</v>
       </c>
       <c r="H25" s="0" t="n">
         <v>880</v>
@@ -4356,22 +4415,22 @@
         <v>25</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>57</v>
+        <v>9</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>31</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>520</v>
@@ -4382,22 +4441,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>60</v>
+        <v>9</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>34</v>
       </c>
       <c r="H27" s="0" t="n">
         <v>680</v>
@@ -4408,22 +4467,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>47</v>
+        <v>9</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>21</v>
       </c>
       <c r="H28" s="0" t="n">
         <v>1236</v>
@@ -4434,22 +4493,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>51</v>
+        <v>10</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>25</v>
       </c>
       <c r="H29" s="0" t="n">
         <v>1800</v>
@@ -4460,22 +4519,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>57</v>
+        <v>10</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>31</v>
       </c>
       <c r="H30" s="0" t="n">
         <v>1200</v>
@@ -4486,22 +4545,22 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="G31" s="0" t="s">
-        <v>52</v>
+        <v>10</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>26</v>
       </c>
       <c r="H31" s="0" t="n">
         <v>1440</v>
@@ -4529,176 +4588,176 @@
       <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>211</v>
+      </c>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="F15" s="2"/>
+        <v>212</v>
+      </c>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>212</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -4723,70 +4782,70 @@
       <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>222</v>
+        <v>209</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>